<commit_message>
Finish account register user logic. Added some changes for easy testing.
</commit_message>
<xml_diff>
--- a/DriverSchoolsDb.xlsx
+++ b/DriverSchoolsDb.xlsx
@@ -16,6 +16,7 @@
     <sheet name="flow" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -97,7 +98,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="127">
   <si>
     <t>Id</t>
   </si>
@@ -469,6 +470,15 @@
   </si>
   <si>
     <t>Vin</t>
+  </si>
+  <si>
+    <t>Credit card number</t>
+  </si>
+  <si>
+    <t>HireDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -1361,7 +1371,7 @@
   <dimension ref="A1:Z29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1677,7 +1687,12 @@
       <c r="B9" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="F9" s="14"/>
+      <c r="F9" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>125</v>
+      </c>
       <c r="I9" s="57"/>
       <c r="J9" s="14" t="s">
         <v>122</v>
@@ -1795,7 +1810,9 @@
         <v>64</v>
       </c>
       <c r="C14" s="60"/>
-      <c r="I14" s="57"/>
+      <c r="I14" s="57" t="s">
+        <v>126</v>
+      </c>
       <c r="J14" s="57"/>
       <c r="L14" s="57"/>
       <c r="M14" s="57"/>

</xml_diff>

<commit_message>
Update Lesson model for FullCalendar usage. Added Lesson service class and interface. closes #66
</commit_message>
<xml_diff>
--- a/DriverSchoolsDb.xlsx
+++ b/DriverSchoolsDb.xlsx
@@ -16,7 +16,6 @@
     <sheet name="flow" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -98,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="127">
   <si>
     <t>Id</t>
   </si>
@@ -1371,7 +1370,7 @@
   <dimension ref="A1:Z29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1745,12 +1744,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="20" t="s">
         <v>8</v>
       </c>
       <c r="I11" s="57"/>
-      <c r="J11" s="57"/>
+      <c r="J11" s="16" t="s">
+        <v>101</v>
+      </c>
       <c r="L11" s="57"/>
       <c r="M11" s="57"/>
       <c r="N11" s="57"/>

</xml_diff>